<commit_message>
fixed jar lib paths
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="135">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -432,6 +432,9 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>

</xml_diff>